<commit_message>
edit page acceuil & dashboard
</commit_message>
<xml_diff>
--- a/Sprint2/Burndown_Chart.xlsx
+++ b/Sprint2/Burndown_Chart.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t xml:space="preserve">Burndown Chart </t>
   </si>
@@ -827,8 +827,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.317766119090622"/>
-          <c:y val="0.0958409654132098"/>
+          <c:x val="0.317787014476136"/>
+          <c:y val="0.0958461289801196"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -846,10 +846,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.118975946790516"/>
-          <c:y val="0.10284452106454"/>
-          <c:w val="0.863937387116195"/>
-          <c:h val="0.784775347484107"/>
+          <c:x val="0.118962304715494"/>
+          <c:y val="0.102850061957869"/>
+          <c:w val="0.863924322774832"/>
+          <c:h val="0.784709875545499"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -937,22 +937,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v/>
@@ -975,8 +975,8 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="0"/>
-        <c:axId val="27087243"/>
-        <c:axId val="20694801"/>
+        <c:axId val="49897572"/>
+        <c:axId val="80719384"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1073,22 +1073,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v/>
@@ -1218,22 +1218,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v/>
@@ -1263,11 +1263,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="31513924"/>
-        <c:axId val="50775180"/>
+        <c:axId val="5044734"/>
+        <c:axId val="86459765"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="27087243"/>
+        <c:axId val="49897572"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,14 +1333,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20694801"/>
+        <c:crossAx val="80719384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20694801"/>
+        <c:axId val="80719384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1377,8 +1377,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0372122358877326"/>
-              <c:y val="0.382124771037604"/>
+              <c:x val="0.0372079690411352"/>
+              <c:y val="0.38203760573245"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1412,11 +1412,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27087243"/>
+        <c:crossAx val="49897572"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="31513924"/>
+        <c:axId val="5044734"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,14 +1482,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50775180"/>
+        <c:crossAx val="86459765"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50775180"/>
+        <c:axId val="86459765"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1526,8 +1526,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0372122358877326"/>
-              <c:y val="0.382124771037604"/>
+              <c:x val="0.0372079690411352"/>
+              <c:y val="0.38203760573245"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1561,7 +1561,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31513924"/>
+        <c:crossAx val="5044734"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1631,9 +1631,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>393120</xdr:colOff>
+      <xdr:colOff>392760</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1642,8 +1642,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3484440" y="4485240"/>
-          <a:ext cx="6620040" cy="1776960"/>
+          <a:off x="3485160" y="4485240"/>
+          <a:ext cx="6619680" cy="1776600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1764,15 +1764,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>993240</xdr:colOff>
+      <xdr:colOff>992520</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>87120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1015920</xdr:colOff>
+      <xdr:colOff>1014840</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1782,7 +1782,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="6548760" y="6371640"/>
-          <a:ext cx="2902320" cy="5827320"/>
+          <a:ext cx="2901960" cy="5826960"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1827,9 +1827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>990720</xdr:colOff>
+      <xdr:colOff>990360</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1838,8 +1838,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3014640" y="7011720"/>
-          <a:ext cx="6411240" cy="373680"/>
+          <a:off x="3015360" y="7011720"/>
+          <a:ext cx="6410880" cy="373320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1891,13 +1891,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>49680</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1455120</xdr:colOff>
+      <xdr:colOff>1454760</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1906,8 +1906,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="4535640" y="7576200"/>
-          <a:ext cx="2475000" cy="2103840"/>
+          <a:off x="4536360" y="7575480"/>
+          <a:ext cx="2474640" cy="2103480"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1952,9 +1952,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>660600</xdr:colOff>
+      <xdr:colOff>660240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1007280</xdr:rowOff>
+      <xdr:rowOff>1006920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1968,7 +1968,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="343080" y="343080"/>
-          <a:ext cx="3115080" cy="664200"/>
+          <a:ext cx="3115440" cy="663840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1989,9 +1989,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>660240</xdr:colOff>
+      <xdr:colOff>659880</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2000,8 +2000,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3078000" y="8640360"/>
-          <a:ext cx="6017400" cy="396360"/>
+          <a:off x="3078720" y="8640360"/>
+          <a:ext cx="6017040" cy="396000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2057,9 +2057,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1798920</xdr:colOff>
+      <xdr:colOff>1798560</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2068,8 +2068,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="4802400" y="8779320"/>
-          <a:ext cx="2552040" cy="857160"/>
+          <a:off x="4803120" y="8779320"/>
+          <a:ext cx="2551680" cy="856800"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2114,9 +2114,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>470160</xdr:colOff>
+      <xdr:colOff>469800</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2124,8 +2124,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10422720" y="1336320"/>
-        <a:ext cx="12556800" cy="6681960"/>
+        <a:off x="10423440" y="1336320"/>
+        <a:ext cx="12558240" cy="6681600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2144,9 +2144,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>217440</xdr:colOff>
+      <xdr:colOff>217080</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2155,8 +2155,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19717560" y="4285080"/>
-          <a:ext cx="1951200" cy="203040"/>
+          <a:off x="19718280" y="4285080"/>
+          <a:ext cx="1951920" cy="202680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2207,15 +2207,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1068120</xdr:colOff>
+      <xdr:colOff>1068480</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>165240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>570600</xdr:colOff>
+      <xdr:colOff>570240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2224,8 +2224,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6705360" y="165240"/>
-          <a:ext cx="4837320" cy="1015200"/>
+          <a:off x="6705720" y="165240"/>
+          <a:ext cx="4836600" cy="1014840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2274,13 +2274,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>101880</xdr:colOff>
+      <xdr:colOff>101520</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>139680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>914040</xdr:colOff>
+      <xdr:colOff>913320</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
@@ -2291,8 +2291,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5739120" y="977760"/>
-          <a:ext cx="812160" cy="360"/>
+          <a:off x="5738760" y="977760"/>
+          <a:ext cx="811800" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2333,13 +2333,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>152280</xdr:colOff>
       <xdr:row>163</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
+      <xdr:rowOff>93240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>508320</xdr:colOff>
       <xdr:row>167</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2348,8 +2348,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1221480" y="3951000"/>
-          <a:ext cx="4924080" cy="736920"/>
+          <a:off x="1221480" y="3954960"/>
+          <a:ext cx="4924080" cy="736560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2415,16 +2415,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>-218520</xdr:colOff>
-      <xdr:row>159</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>713160</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>93240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1728360</xdr:colOff>
-      <xdr:row>166</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>214920</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2432,66 +2432,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="-218520" y="3074760"/>
-          <a:ext cx="3016080" cy="1459800"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="28440">
-          <a:solidFill>
-            <a:srgbClr val="244d80"/>
-          </a:solidFill>
-          <a:miter/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>712800</xdr:colOff>
-      <xdr:row>163</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>215280</xdr:colOff>
-      <xdr:row>167</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
         <a:xfrm>
-          <a:off x="6350040" y="3951000"/>
-          <a:ext cx="4837320" cy="736920"/>
+          <a:off x="6350400" y="3954960"/>
+          <a:ext cx="4836600" cy="736560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2584,26 +2527,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1947240</xdr:colOff>
-      <xdr:row>159</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>803160</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>441360</xdr:colOff>
-      <xdr:row>166</xdr:row>
-      <xdr:rowOff>178560</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1947600</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="CustomShape 1"/>
+        <xdr:cNvPr id="13" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7584480" y="3075120"/>
-          <a:ext cx="5712840" cy="1561680"/>
+          <a:off x="1872360" y="1517040"/>
+          <a:ext cx="5712480" cy="1561320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2642,25 +2585,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2186280</xdr:colOff>
-      <xdr:row>159</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:colOff>2150280</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2222280</xdr:colOff>
-      <xdr:row>166</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:colOff>2185920</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CustomShape 1"/>
+        <xdr:cNvPr id="14" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="7823520" y="3074760"/>
-          <a:ext cx="36000" cy="1523160"/>
+          <a:off x="7787520" y="1555920"/>
+          <a:ext cx="35640" cy="1522800"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2698,26 +2641,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1044000</xdr:colOff>
-      <xdr:row>159</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>811800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>184320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2565000</xdr:colOff>
-      <xdr:row>166</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1043640</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvPr id="15" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="4507200" y="3075120"/>
-          <a:ext cx="3695040" cy="1427760"/>
+          <a:off x="811800" y="1650960"/>
+          <a:ext cx="3695040" cy="1427400"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2758,23 +2701,23 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1447920</xdr:colOff>
       <xdr:row>163</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>105840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>153000</xdr:colOff>
+      <xdr:colOff>152640</xdr:colOff>
       <xdr:row>167</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="CustomShape 1"/>
+        <xdr:cNvPr id="16" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12420000" y="3963600"/>
-          <a:ext cx="7890840" cy="736920"/>
+          <a:off x="12420000" y="3967560"/>
+          <a:ext cx="7891200" cy="736560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2823,25 +2766,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1333440</xdr:colOff>
-      <xdr:row>159</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:colOff>1297440</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1369800</xdr:colOff>
-      <xdr:row>167</xdr:row>
-      <xdr:rowOff>55080</xdr:rowOff>
+      <xdr:colOff>1333440</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="CustomShape 1"/>
+        <xdr:cNvPr id="17" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="15258960" y="3075120"/>
-          <a:ext cx="36360" cy="1638000"/>
+          <a:off x="15222960" y="1440720"/>
+          <a:ext cx="36000" cy="1637640"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2886,13 +2829,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>38160</xdr:colOff>
+      <xdr:colOff>37800</xdr:colOff>
       <xdr:row>170</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Grafik 13" descr=""/>
+        <xdr:cNvPr id="18" name="Grafik 13" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2901,8 +2844,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16852680" y="5052600"/>
-          <a:ext cx="2285640" cy="380160"/>
+          <a:off x="16852680" y="5056560"/>
+          <a:ext cx="2285280" cy="379800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2922,19 +2865,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>977760</xdr:colOff>
+      <xdr:colOff>978120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>12240</xdr:colOff>
+      <xdr:colOff>11880</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Grafik 13" descr=""/>
+        <xdr:cNvPr id="19" name="Grafik 13" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2943,8 +2886,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4259160" y="3229920"/>
-          <a:ext cx="2411640" cy="379080"/>
+          <a:off x="4259520" y="3173040"/>
+          <a:ext cx="2410920" cy="378720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3030,8 +2973,8 @@
   </sheetPr>
   <dimension ref="A1:AT58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3051,7 +2994,9 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="n">
+        <v>22</v>
+      </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -3130,7 +3075,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>44362</v>
+        <v>44369</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="12" t="s">
@@ -3138,7 +3083,7 @@
       </c>
       <c r="E5" s="13" t="n">
         <f aca="false">B5+B6</f>
-        <v>44368</v>
+        <v>44375</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="1"/>
@@ -3211,7 +3156,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="20" t="n">
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -3234,9 +3179,9 @@
       <c r="D9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="20" t="n">
+      <c r="E9" s="20" t="e">
         <f aca="false">E8-'Auxiliaire - Tableau Burndown'!$D$15</f>
-        <v>11</v>
+        <v>#N/A</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -4096,7 +4041,7 @@
   <dimension ref="A1:AK199"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4121,7 +4066,7 @@
       </c>
       <c r="C1" s="31" t="n">
         <f aca="false">'Vue d''ensemble'!$B$5</f>
-        <v>44362</v>
+        <v>44369</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -4237,7 +4182,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="40" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>1</v>
@@ -4245,22 +4190,20 @@
       <c r="E6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="F6" s="10"/>
       <c r="G6" s="31" t="n">
-        <v>44363</v>
+        <v>44369</v>
       </c>
       <c r="H6" s="41" t="n">
         <f aca="false">IF(ISBLANK(Backlog!$G6),"",Backlog!$G6-$C$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="10" t="str">
         <f aca="false">IF(ISBLANK(Backlog!$G6),"n","y")</f>
         <v>y</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
         <v>1</v>
       </c>
@@ -4268,28 +4211,26 @@
         <v>2</v>
       </c>
       <c r="C7" s="40" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D7" s="10" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="F7" s="10"/>
       <c r="G7" s="42" t="n">
-        <v>44364</v>
+        <v>44370</v>
       </c>
       <c r="H7" s="41" t="n">
         <f aca="false">IF(ISBLANK(Backlog!$G7),"",Backlog!$G7-$C$1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="10" t="str">
         <f aca="false">IF(ISBLANK(Backlog!$G7),"n","y")</f>
         <v>y</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
         <v>1</v>
       </c>
@@ -4297,28 +4238,26 @@
         <v>3</v>
       </c>
       <c r="C8" s="40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="10" t="n">
         <v>3</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="F8" s="10"/>
       <c r="G8" s="42" t="n">
-        <v>44365</v>
+        <v>44371</v>
       </c>
       <c r="H8" s="41" t="n">
         <f aca="false">IF(ISBLANK(Backlog!$G8),"",Backlog!$G8-$C$1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" s="10" t="str">
         <f aca="false">IF(ISBLANK(Backlog!$G8),"n","y")</f>
         <v>y</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
         <v>1</v>
       </c>
@@ -4332,22 +4271,20 @@
         <v>4</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="F9" s="10"/>
       <c r="G9" s="42" t="n">
-        <v>44366</v>
+        <v>44372</v>
       </c>
       <c r="H9" s="41" t="n">
         <f aca="false">IF(ISBLANK(Backlog!$G9),"",Backlog!$G9-$C$1)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I9" s="10" t="str">
         <f aca="false">IF(ISBLANK(Backlog!$G9),"n","y")</f>
         <v>y</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="n">
         <v>1</v>
       </c>
@@ -4363,7 +4300,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="42" t="n">
-        <v>44368</v>
+        <v>44375</v>
       </c>
       <c r="H10" s="41" t="n">
         <v>5</v>
@@ -4373,10 +4310,12 @@
         <v>y</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="40"/>
+      <c r="C11" s="40" t="n">
+        <v>1</v>
+      </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -6899,7 +6838,7 @@
       <c r="B160" s="44"/>
       <c r="C160" s="44" t="n">
         <f aca="false">SUBTOTAL(109,Backlog!$C$6:$C$159)</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D160" s="44"/>
       <c r="E160" s="44"/>
@@ -7371,7 +7310,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7416,130 +7355,124 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="41" t="n">
-        <f aca="false">Backlog!$C$160-(Backlog!$C$160/'Vue d''ensemble'!$E$6*'Auxiliaire - Tableau Burndown'!$A4)</f>
-        <v>16</v>
+      <c r="B4" s="40" t="n">
+        <v>6</v>
       </c>
       <c r="C4" s="10" t="n">
         <f aca="false">Backlog!$C$160</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D4" s="10" t="n">
         <f aca="false">IF('Auxiliaire - Tableau Burndown'!$E4="y",SUMIF(Backlog!$H$6:$H$159,'Auxiliaire - Tableau Burndown'!$A4,Backlog!$C$6:$C$159),#N/A)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E4" s="10" t="str">
         <f aca="true">IF(NOW()&gt;=Backlog!$C$1+'Auxiliaire - Tableau Burndown'!$A4,"y","n")</f>
         <v>y</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="41" t="n">
-        <f aca="false">Backlog!$C$160-(Backlog!$C$160/'Vue d''ensemble'!$E$6*'Auxiliaire - Tableau Burndown'!$A5)</f>
-        <v>12.8</v>
+      <c r="B5" s="40" t="n">
+        <v>5</v>
       </c>
       <c r="C5" s="10" t="n">
         <f aca="false">C4-'Auxiliaire - Tableau Burndown'!$D5</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D5" s="10" t="n">
         <f aca="false">IF('Auxiliaire - Tableau Burndown'!$E5="y",SUMIF(Backlog!$H$6:$H$159,'Auxiliaire - Tableau Burndown'!$A5,Backlog!$C$6:$C$159),#N/A)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="10" t="str">
         <f aca="true">IF(NOW()&gt;=Backlog!$C$1+'Auxiliaire - Tableau Burndown'!$A5,"y","n")</f>
         <v>y</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="41" t="n">
-        <f aca="false">Backlog!$C$160-(Backlog!$C$160/'Vue d''ensemble'!$E$6*'Auxiliaire - Tableau Burndown'!$A6)</f>
-        <v>9.6</v>
-      </c>
-      <c r="C6" s="10" t="n">
+      <c r="B6" s="40" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="e">
         <f aca="false">C5-'Auxiliaire - Tableau Burndown'!$D6</f>
-        <v>10</v>
-      </c>
-      <c r="D6" s="10" t="n">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" s="10" t="e">
         <f aca="false">IF('Auxiliaire - Tableau Burndown'!$E6="y",SUMIF(Backlog!$H$6:$H$159,'Auxiliaire - Tableau Burndown'!$A6,Backlog!$C$6:$C$159),#N/A)</f>
-        <v>2</v>
+        <v>#N/A</v>
       </c>
       <c r="E6" s="10" t="str">
         <f aca="true">IF(NOW()&gt;=Backlog!$C$1+'Auxiliaire - Tableau Burndown'!$A6,"y","n")</f>
-        <v>y</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>n</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="41" t="n">
-        <f aca="false">Backlog!$C$160-(Backlog!$C$160/'Vue d''ensemble'!$E$6*'Auxiliaire - Tableau Burndown'!$A7)</f>
-        <v>6.4</v>
-      </c>
-      <c r="C7" s="10" t="n">
+      <c r="B7" s="40" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10" t="e">
         <f aca="false">C6-'Auxiliaire - Tableau Burndown'!$D7</f>
-        <v>5</v>
-      </c>
-      <c r="D7" s="10" t="n">
+        <v>#N/A</v>
+      </c>
+      <c r="D7" s="10" t="e">
         <f aca="false">IF('Auxiliaire - Tableau Burndown'!$E7="y",SUMIF(Backlog!$H$6:$H$159,'Auxiliaire - Tableau Burndown'!$A7,Backlog!$C$6:$C$159),#N/A)</f>
-        <v>5</v>
+        <v>#N/A</v>
       </c>
       <c r="E7" s="10" t="str">
         <f aca="true">IF(NOW()&gt;=Backlog!$C$1+'Auxiliaire - Tableau Burndown'!$A7,"y","n")</f>
-        <v>y</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>n</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="41" t="n">
-        <f aca="false">Backlog!$C$160-(Backlog!$C$160/'Vue d''ensemble'!$E$6*'Auxiliaire - Tableau Burndown'!$A8)</f>
-        <v>3.2</v>
-      </c>
-      <c r="C8" s="10" t="n">
+      <c r="B8" s="40" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10" t="e">
         <f aca="false">C7-'Auxiliaire - Tableau Burndown'!$D8</f>
-        <v>2</v>
-      </c>
-      <c r="D8" s="10" t="n">
+        <v>#N/A</v>
+      </c>
+      <c r="D8" s="10" t="e">
         <f aca="false">IF('Auxiliaire - Tableau Burndown'!$E8="y",SUMIF(Backlog!$H$6:$H$159,'Auxiliaire - Tableau Burndown'!$A8,Backlog!$C$6:$C$159),#N/A)</f>
-        <v>3</v>
+        <v>#N/A</v>
       </c>
       <c r="E8" s="10" t="str">
         <f aca="true">IF(NOW()&gt;=Backlog!$C$1+'Auxiliaire - Tableau Burndown'!$A8,"y","n")</f>
-        <v>y</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>n</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="41" t="n">
-        <f aca="false">Backlog!$C$160-(Backlog!$C$160/'Vue d''ensemble'!$E$6*'Auxiliaire - Tableau Burndown'!$A9)</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="10" t="n">
+      <c r="B9" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10" t="e">
         <f aca="false">C8-'Auxiliaire - Tableau Burndown'!$D9</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="10" t="n">
+        <v>#N/A</v>
+      </c>
+      <c r="D9" s="10" t="e">
         <f aca="false">IF('Auxiliaire - Tableau Burndown'!$E9="y",SUMIF(Backlog!$H$6:$H$159,'Auxiliaire - Tableau Burndown'!$A9,Backlog!$C$6:$C$159),#N/A)</f>
-        <v>2</v>
+        <v>#N/A</v>
       </c>
       <c r="E9" s="10" t="str">
         <f aca="true">IF(NOW()&gt;=Backlog!$C$1+'Auxiliaire - Tableau Burndown'!$A9,"y","n")</f>
-        <v>y</v>
+        <v>n</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7598,9 +7531,9 @@
       </c>
       <c r="B15" s="41"/>
       <c r="C15" s="10"/>
-      <c r="D15" s="10" t="n">
+      <c r="D15" s="10" t="e">
         <f aca="false">SUMIFS('Auxiliaire - Tableau Burndown'!$D$4:$D$14,'Auxiliaire - Tableau Burndown'!$D$4:$D$14,"&lt;&gt;#NV")</f>
-        <v>16</v>
+        <v>#N/A</v>
       </c>
       <c r="E15" s="10" t="n">
         <f aca="false">SUBTOTAL(103,'Auxiliaire - Tableau Burndown'!$E$4:$E$14)</f>

</xml_diff>